<commit_message>
can upload inventory and rma to arango
</commit_message>
<xml_diff>
--- a/example/eO/data/Habnet_sortie_case_1.xlsx
+++ b/example/eO/data/Habnet_sortie_case_1.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desho/CORAL-eO/example/eO/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B31EA-2409-0E4A-A0C7-80267D80795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -19,9 +28,6 @@
     <t>Subassembly</t>
   </si>
   <si>
-    <t>Initial Count</t>
-  </si>
-  <si>
     <t>M (kg)</t>
   </si>
   <si>
@@ -31,9 +37,6 @@
     <t>MTBF (h)</t>
   </si>
   <si>
-    <t># in Pmry.</t>
-  </si>
-  <si>
     <t># of Spares</t>
   </si>
   <si>
@@ -182,66 +185,85 @@
   </si>
   <si>
     <t>Support Structure</t>
+  </si>
+  <si>
+    <t># in Pmry</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -431,23 +453,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="32.86"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,22 +482,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -489,35 +516,35 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>10.89</v>
       </c>
       <c r="E2" s="3">
-        <v>0.0045</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="F2" s="3">
-        <v>156200.0</v>
+        <v>156200</v>
       </c>
       <c r="G2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3">
         <v>5.58</v>
@@ -526,15 +553,15 @@
         <v>0.03</v>
       </c>
       <c r="F3" s="3">
-        <v>129700.0</v>
+        <v>129700</v>
       </c>
       <c r="G3" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3">
         <v>39.92</v>
@@ -543,191 +570,191 @@
         <v>0.1784</v>
       </c>
       <c r="F4" s="3">
-        <v>32900.0</v>
+        <v>32900</v>
       </c>
       <c r="G4" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
         <v>42.64</v>
       </c>
       <c r="E5" s="3">
-        <v>0.085</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F5" s="3">
-        <v>77100.0</v>
+        <v>77100</v>
       </c>
       <c r="G5" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3">
         <v>3.31</v>
       </c>
       <c r="E6" s="3">
-        <v>0.0085</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="F6" s="3">
-        <v>242700.0</v>
+        <v>242700</v>
       </c>
       <c r="G6" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>5.58</v>
       </c>
       <c r="E7" s="3">
-        <v>0.0255</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="F7" s="3">
-        <v>129700.0</v>
+        <v>129700</v>
       </c>
       <c r="G7" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>2.72</v>
       </c>
       <c r="E8" s="3">
-        <v>0.0057</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="F8" s="3">
-        <v>2270000.0</v>
+        <v>2270000</v>
       </c>
       <c r="G8" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3">
         <v>3.04</v>
       </c>
       <c r="E9" s="3">
-        <v>0.0017</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="F9" s="3">
-        <v>117000.0</v>
+        <v>117000</v>
       </c>
       <c r="G9" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3">
         <v>42.64</v>
       </c>
       <c r="E10" s="3">
-        <v>0.085</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>77100.0</v>
+        <v>77100</v>
       </c>
       <c r="G10" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3">
         <v>49.71</v>
       </c>
       <c r="E11" s="3">
-        <v>0.3933</v>
+        <v>0.39329999999999998</v>
       </c>
       <c r="F11" s="3">
-        <v>832600.0</v>
+        <v>832600</v>
       </c>
       <c r="G11" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3">
         <v>4.04</v>
       </c>
       <c r="E12" s="3">
-        <v>0.0173</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="F12" s="3">
-        <v>2350000.0</v>
+        <v>2350000</v>
       </c>
       <c r="G12" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3">
         <v>0.45</v>
       </c>
       <c r="E13" s="3">
-        <v>2.0E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="F13" s="3">
-        <v>1250000.0</v>
+        <v>1250000</v>
       </c>
       <c r="G13" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3">
         <v>0.64</v>
       </c>
       <c r="E14" s="3">
-        <v>6.0E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="F14" s="3">
-        <v>1140000.0</v>
+        <v>1140000</v>
       </c>
       <c r="G14" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3">
         <v>25.31</v>
@@ -736,211 +763,211 @@
         <v>0.1308</v>
       </c>
       <c r="F15" s="3">
-        <v>333000.0</v>
+        <v>333000</v>
       </c>
       <c r="G15" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="3">
         <v>0.48</v>
       </c>
       <c r="E16" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>1250000.0</v>
+        <v>1250000</v>
       </c>
       <c r="G16" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3">
         <v>7.45</v>
       </c>
       <c r="E17" s="3">
-        <v>0.0071</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="F17" s="3">
-        <v>32900.0</v>
+        <v>32900</v>
       </c>
       <c r="G17" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C18" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="3">
         <v>0.26</v>
       </c>
       <c r="E18" s="3">
-        <v>0.0014</v>
+        <v>1.4E-3</v>
       </c>
       <c r="F18" s="3">
-        <v>3.76E7</v>
+        <v>37600000</v>
       </c>
       <c r="G18" s="3">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3">
         <v>11.93</v>
       </c>
       <c r="E19" s="3">
-        <v>0.0583</v>
+        <v>5.8299999999999998E-2</v>
       </c>
       <c r="F19" s="3">
-        <v>131000.0</v>
+        <v>131000</v>
       </c>
       <c r="G19" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3">
         <v>0.64</v>
       </c>
       <c r="E20" s="3">
-        <v>6.0E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="F20" s="3">
-        <v>1140000.0</v>
+        <v>1140000</v>
       </c>
       <c r="G20" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D21" s="3">
         <v>78.05</v>
       </c>
       <c r="E21" s="3">
-        <v>3.3808</v>
+        <v>3.3807999999999998</v>
       </c>
       <c r="F21" s="3">
-        <v>242700.0</v>
+        <v>242700</v>
       </c>
       <c r="G21" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="4">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3">
         <v>58.56</v>
       </c>
       <c r="E22" s="3">
-        <v>3.942</v>
+        <v>3.9420000000000002</v>
       </c>
       <c r="G22" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3">
-        <v>36.52</v>
+        <v>36.520000000000003</v>
       </c>
       <c r="E23" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="G23" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3">
         <v>200.07</v>
       </c>
       <c r="E24" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F24" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="G24" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C25" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="3">
         <v>11.38</v>
       </c>
       <c r="E25" s="3">
-        <v>0.1463</v>
+        <v>0.14630000000000001</v>
       </c>
       <c r="F25" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="G25" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C26" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3">
         <v>0.02</v>
       </c>
       <c r="E26" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F26" s="3">
-        <v>138408.0</v>
+        <v>138408</v>
       </c>
       <c r="G26" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C27" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3">
         <v>6.03</v>
@@ -949,286 +976,286 @@
         <v>0.1186</v>
       </c>
       <c r="G27" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C28" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28" s="3">
         <v>37.81</v>
       </c>
       <c r="E28" s="3">
-        <v>0.8551</v>
+        <v>0.85509999999999997</v>
       </c>
       <c r="F28" s="3">
-        <v>832600.0</v>
+        <v>832600</v>
       </c>
       <c r="G28" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C29" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="3">
-        <v>2.18</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E29" s="3">
-        <v>0.0082</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="F29" s="3">
         <v>296701.2</v>
       </c>
       <c r="G29" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3">
         <v>34.61</v>
       </c>
       <c r="E30" s="3">
-        <v>0.0726</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="F30" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="G30" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C31" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="3">
         <v>83.02</v>
       </c>
       <c r="E31" s="3">
-        <v>0.4906</v>
+        <v>0.49059999999999998</v>
       </c>
       <c r="G31" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="3">
         <v>47.43</v>
       </c>
       <c r="E32" s="3">
-        <v>0.0045</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="F32" s="3">
-        <v>27156.0</v>
+        <v>27156</v>
       </c>
       <c r="G32" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="4">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D33" s="3">
         <v>5.71</v>
       </c>
       <c r="E33" s="3">
-        <v>0.0119</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="F33" s="3">
-        <v>27156.0</v>
+        <v>27156</v>
       </c>
       <c r="G33" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C34" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="3">
         <v>14.44</v>
       </c>
       <c r="E34" s="3">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F34" s="3">
-        <v>98112.0</v>
+        <v>98112</v>
       </c>
       <c r="G34" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35" s="3">
         <v>2.16</v>
       </c>
       <c r="E35" s="3">
-        <v>7.0E-4</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="F35" s="3">
-        <v>144540.0</v>
+        <v>144540</v>
       </c>
       <c r="G35" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3">
         <v>20.78</v>
       </c>
       <c r="E36" s="3">
-        <v>0.4181</v>
+        <v>0.41810000000000003</v>
       </c>
       <c r="F36" s="3">
-        <v>50000.0</v>
+        <v>50000</v>
       </c>
       <c r="G36" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C37" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D37" s="3">
         <v>0.24</v>
       </c>
       <c r="E37" s="3">
-        <v>0.0097</v>
+        <v>9.7000000000000003E-3</v>
       </c>
       <c r="F37" s="3">
-        <v>131000.0</v>
+        <v>131000</v>
       </c>
       <c r="G37" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C38" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D38" s="3">
         <v>0.53</v>
       </c>
       <c r="E38" s="3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F38" s="3">
-        <v>832600.0</v>
+        <v>832600</v>
       </c>
       <c r="G38" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D39" s="3">
         <v>0.53</v>
       </c>
       <c r="E39" s="3">
-        <v>0.0064</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="F39" s="3">
-        <v>77100.0</v>
+        <v>77100</v>
       </c>
       <c r="G39" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C40" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D40" s="3">
-        <v>8.04</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="E40" s="3">
-        <v>0.0465</v>
+        <v>4.65E-2</v>
       </c>
       <c r="F40" s="3">
         <v>66666.7</v>
       </c>
       <c r="G40" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H40" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C41" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D41" s="3">
         <v>3.1</v>
       </c>
       <c r="E41" s="3">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="F41" s="3">
-        <v>500000.0</v>
+        <v>500000</v>
       </c>
       <c r="G41" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H41" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C42" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D42" s="3">
         <v>3.45</v>
       </c>
       <c r="G42" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>